<commit_message>
Project Import testcase passed.
</commit_message>
<xml_diff>
--- a/Excel/Project.xlsx
+++ b/Excel/Project.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Praful_Personal\GitProject\AutomationTestScript\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nayan.thakor\Documents\PersonalWorkspace\AMPS_Automation_V2\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674695F4-1677-4B16-8386-FA363C4E99E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectGroup" sheetId="21" r:id="rId1"/>
@@ -21,14 +22,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -171,9 +164,6 @@
     <t>AddDocumentVersionROW</t>
   </si>
   <si>
-    <t>10# Land Data$'</t>
-  </si>
-  <si>
     <t>WorkSheet</t>
   </si>
   <si>
@@ -204,19 +194,22 @@
     <t>Parcel Import</t>
   </si>
   <si>
-    <t>10 Parcel Import$'</t>
-  </si>
-  <si>
     <t>Alt Test Automation Demo 01_ROW</t>
   </si>
   <si>
     <t>10 Parcel Import</t>
+  </si>
+  <si>
+    <t>10# Land Data$</t>
+  </si>
+  <si>
+    <t>10 Parcel Import$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -560,7 +553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -651,7 +644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -971,36 +964,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E6" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
-    <hyperlink ref="F7" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -1028,67 +1021,67 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
       <c r="D5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>